<commit_message>
chore: deploy all pending changes
</commit_message>
<xml_diff>
--- a/templates/counteragent_import_template.xlsx
+++ b/templates/counteragent_import_template.xlsx
@@ -8,17 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\next-postgres-starter\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6683032D-268E-4864-8CE1-A73D84FB1159}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26FED92D-32FF-4496-A7B1-95FD850F8A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Counteragent" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId1"/>
+    <sheet name="Counteragent_new" sheetId="3" r:id="rId2"/>
+    <sheet name="Counteragent" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Counteragent!$A$1:$AA$277</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$AC$280</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Counteragent!$A$1:$AA$277</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Counteragent_new!$A$1:$Z$67</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sheet1!$A$1:$AC$280</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet3!$A$1:$E$67</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,8 +42,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5024" uniqueCount="1647">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5422" uniqueCount="1793">
   <si>
     <t>ts</t>
   </si>
@@ -4983,13 +5009,451 @@
   </si>
   <si>
     <t>0ef7c94f-b314-492e-8090-d5a8a9b74681</t>
+  </si>
+  <si>
+    <t>CODE</t>
+  </si>
+  <si>
+    <t>IBAN</t>
+  </si>
+  <si>
+    <t>ENTITY TYPE</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>GE96BG0000000730563700GEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">შპს </t>
+  </si>
+  <si>
+    <t>გეა ნოვა</t>
+  </si>
+  <si>
+    <t>GE24TB7236936020100010</t>
+  </si>
+  <si>
+    <t>ჯი თი სი რენთ</t>
+  </si>
+  <si>
+    <t>GE84BG0000000100756011GEL</t>
+  </si>
+  <si>
+    <t>ტოროსიანი მარინა</t>
+  </si>
+  <si>
+    <t>GE05BS0000000010936920</t>
+  </si>
+  <si>
+    <t>GE26BG0000000528006165GEL</t>
+  </si>
+  <si>
+    <t>C01492631</t>
+  </si>
+  <si>
+    <t>GE92BG0000000609672187GEL</t>
+  </si>
+  <si>
+    <t>აანდიყევ ალასგარ</t>
+  </si>
+  <si>
+    <t>GE07BG0000000523441105GEL</t>
+  </si>
+  <si>
+    <t>ნიკოლას</t>
+  </si>
+  <si>
+    <t>ES7500815094800001135224</t>
+  </si>
+  <si>
+    <t>Hidral</t>
+  </si>
+  <si>
+    <t>GE84BG0000000161360738GEL</t>
+  </si>
+  <si>
+    <t>ტეკი</t>
+  </si>
+  <si>
+    <t>აი ეს ბი ეიჩ</t>
+  </si>
+  <si>
+    <t>445612864</t>
+  </si>
+  <si>
+    <t>GE80BG0000000498659686GEL</t>
+  </si>
+  <si>
+    <t>მორჩილაძე მარიანა</t>
+  </si>
+  <si>
+    <t>GE52BG0000000606293330GEL</t>
+  </si>
+  <si>
+    <t>რობირენტ.ჯი</t>
+  </si>
+  <si>
+    <t>GE82BG0000000541362251GEL</t>
+  </si>
+  <si>
+    <t>იზორია გიორგი</t>
+  </si>
+  <si>
+    <t>GE54BG0000000162677471GEL</t>
+  </si>
+  <si>
+    <t>ტარიელაძე თეიმურაზ</t>
+  </si>
+  <si>
+    <t>GE13BG0000000534065989GEL</t>
+  </si>
+  <si>
+    <t>ამირან წაქაძე</t>
+  </si>
+  <si>
+    <t>GE83BG0000000548350598GEL</t>
+  </si>
+  <si>
+    <t>სტატუსი</t>
+  </si>
+  <si>
+    <t>GE93BG0000000538027969GEL</t>
+  </si>
+  <si>
+    <t>უნივერსალური ნათება</t>
+  </si>
+  <si>
+    <t>GE02BG0000000622833700GEL</t>
+  </si>
+  <si>
+    <t>ლაცა 2009</t>
+  </si>
+  <si>
+    <t>GE63BG0000000606154034GEL</t>
+  </si>
+  <si>
+    <t>ჩექ ქარ ჯეორჯია</t>
+  </si>
+  <si>
+    <t>GE52BG0000000594459718GEL</t>
+  </si>
+  <si>
+    <t>GE38BG0000000101462223GEL</t>
+  </si>
+  <si>
+    <t>ირემაშვილი აკაკი</t>
+  </si>
+  <si>
+    <t>GE26TB7212436050100001</t>
+  </si>
+  <si>
+    <t>თრეიდერი</t>
+  </si>
+  <si>
+    <t>GE31BG0000000162627833GEL</t>
+  </si>
+  <si>
+    <t>მჟავია დარეჯან</t>
+  </si>
+  <si>
+    <t>GE41BG0000000346051064GEL</t>
+  </si>
+  <si>
+    <t>ქებურია ნიკა</t>
+  </si>
+  <si>
+    <t>GE52BG0000000808306500GEL</t>
+  </si>
+  <si>
+    <t>კორთხონჯია დავით</t>
+  </si>
+  <si>
+    <t>GE37BG0000000131254142GEL</t>
+  </si>
+  <si>
+    <t>კორთხონჯია ზურაბ</t>
+  </si>
+  <si>
+    <t>GE56BG0000000366036092GEL</t>
+  </si>
+  <si>
+    <t>მამულაშვილი შალვა</t>
+  </si>
+  <si>
+    <t>GE52BG0000000101309875GEL</t>
+  </si>
+  <si>
+    <t>ფუტკარაძე გივი</t>
+  </si>
+  <si>
+    <t>GE36BG0000000584703164GEL</t>
+  </si>
+  <si>
+    <t>შერვაშიძე ერეკლე</t>
+  </si>
+  <si>
+    <t>GE29TB7598345064300061</t>
+  </si>
+  <si>
+    <t>მარინა ტოროსიანი</t>
+  </si>
+  <si>
+    <t>GE97TB7713036060100001</t>
+  </si>
+  <si>
+    <t>არბო 2009</t>
+  </si>
+  <si>
+    <t>GE08BG0000000366075562GEL</t>
+  </si>
+  <si>
+    <t>ჯე ფიტტინგ</t>
+  </si>
+  <si>
+    <t>GE60BG0000000537555494GEL</t>
+  </si>
+  <si>
+    <t>ფართი შოპ ჯი</t>
+  </si>
+  <si>
+    <t>GE85TB7151545061100023</t>
+  </si>
+  <si>
+    <t>ჟანა ოგანეზოვი</t>
+  </si>
+  <si>
+    <t>GE05TB7886536080100008</t>
+  </si>
+  <si>
+    <t>იში7788</t>
+  </si>
+  <si>
+    <t>GE21BG0000000759214000GEL</t>
+  </si>
+  <si>
+    <t>ცეცხლაძე როინ</t>
+  </si>
+  <si>
+    <t>GE95BG0000000695964400GEL</t>
+  </si>
+  <si>
+    <t>მურმან გეგია</t>
+  </si>
+  <si>
+    <t>GE57BG0000000215070900GEL</t>
+  </si>
+  <si>
+    <t>ლარისა ფონიავა</t>
+  </si>
+  <si>
+    <t>GE23TB7185636080100003</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ოაგრუპ</t>
+  </si>
+  <si>
+    <t>GE84BG0000000103359782GEL</t>
+  </si>
+  <si>
+    <t>ოთარაშვილი ალექსეი</t>
+  </si>
+  <si>
+    <t>GE08BG0000000312837500GEL</t>
+  </si>
+  <si>
+    <t>კვეზერელი ნიკოლოზ</t>
+  </si>
+  <si>
+    <t>GE87LB0211117682002000</t>
+  </si>
+  <si>
+    <t>სოფიკო ხომასურიძე</t>
+  </si>
+  <si>
+    <t>GE20BG0000000161924296GEL</t>
+  </si>
+  <si>
+    <t>მუკბანიანი ანა</t>
+  </si>
+  <si>
+    <t>GE92BG0000000187220600GEL</t>
+  </si>
+  <si>
+    <t>ბულბულაშვილი ნოდარი</t>
+  </si>
+  <si>
+    <t>GE95TB7931136020100009</t>
+  </si>
+  <si>
+    <t>ნანოტეკ ფროდაქშენ</t>
+  </si>
+  <si>
+    <t>GE20TB7938836020100004</t>
+  </si>
+  <si>
+    <t>ბაგრო ჯორჯია</t>
+  </si>
+  <si>
+    <t>400438371</t>
+  </si>
+  <si>
+    <t>GE94BG0000000654109500GEL</t>
+  </si>
+  <si>
+    <t>ბექაური ქეთევან</t>
+  </si>
+  <si>
+    <t>GE32BG0000000541718947GEL</t>
+  </si>
+  <si>
+    <t>GE37BG0000000610791684GEL</t>
+  </si>
+  <si>
+    <t>ილია ცინცაძე</t>
+  </si>
+  <si>
+    <t>GE50TB7080036060100002</t>
+  </si>
+  <si>
+    <t>ველლი ჯგუფი</t>
+  </si>
+  <si>
+    <t>429336621</t>
+  </si>
+  <si>
+    <t>GE08PC0183600100015821</t>
+  </si>
+  <si>
+    <t>სიდო</t>
+  </si>
+  <si>
+    <t>GE32TB7372336080100012</t>
+  </si>
+  <si>
+    <t>ვერტა ელევატორი</t>
+  </si>
+  <si>
+    <t>GE69TB7863336080100016</t>
+  </si>
+  <si>
+    <t>კოკოსილქ+</t>
+  </si>
+  <si>
+    <t>406320887</t>
+  </si>
+  <si>
+    <t>GE29TB3900000077517777</t>
+  </si>
+  <si>
+    <t>GE29TB7400836010100046</t>
+  </si>
+  <si>
+    <t>ვასილიი კაპლიევ</t>
+  </si>
+  <si>
+    <t>GE73BG0000000279352900GEL</t>
+  </si>
+  <si>
+    <t>მამმადოვ როვშან</t>
+  </si>
+  <si>
+    <t>GE53BG0000000545804791GEL</t>
+  </si>
+  <si>
+    <t>ცანქალ მუამმერ</t>
+  </si>
+  <si>
+    <t>GE88BG0000000499033380GEL</t>
+  </si>
+  <si>
+    <t>უნიკალი</t>
+  </si>
+  <si>
+    <t>GE34TB0600000000609009</t>
+  </si>
+  <si>
+    <t>დიპლომატი</t>
+  </si>
+  <si>
+    <t>EMBASSY OF ISLAMIC REPUBLIC OF IRAN</t>
+  </si>
+  <si>
+    <t>GE11TB1930636080100002</t>
+  </si>
+  <si>
+    <t>GE62TB7183936050100002</t>
+  </si>
+  <si>
+    <t>GE92BG0000000545811849GEL</t>
+  </si>
+  <si>
+    <t>საქსპეცტრანსი</t>
+  </si>
+  <si>
+    <t>GE51BG0000000608679742GEL</t>
+  </si>
+  <si>
+    <t>ხაჭაპურიძე გრიგოლ</t>
+  </si>
+  <si>
+    <t>GE02BG0000000580784491GEL</t>
+  </si>
+  <si>
+    <t>სამხრეთის სამშენებლო კომპანია</t>
+  </si>
+  <si>
+    <t>საქართველოს მცირე და საშუალო საწარმოთა ასოციაცია</t>
+  </si>
+  <si>
+    <t>თორნიკე პაპიაშვილი</t>
+  </si>
+  <si>
+    <t>61007007408</t>
+  </si>
+  <si>
+    <t>0d51a686-652b-478f-9502-50b11abafa54</t>
+  </si>
+  <si>
+    <t>94279771-0dd8-44b8-955b-275714b1489b</t>
+  </si>
+  <si>
+    <t>ნიუ მეტალ ჯორჯია</t>
+  </si>
+  <si>
+    <t>საერთაშორისო სავაჭრო ჯგუფი</t>
+  </si>
+  <si>
+    <t>ოქტო არტჰაუსი</t>
+  </si>
+  <si>
+    <t>ba538574-e93f-4ce8-a780-667b61fc970a</t>
+  </si>
+  <si>
+    <t>ნიკოლოზ ოშხერელი</t>
+  </si>
+  <si>
+    <t>3b6618c9-b4c6-4e78-80e2-442b948fcd64</t>
+  </si>
+  <si>
+    <t>831339ac-64e3-4d4c-9726-074e2d68b19c</t>
+  </si>
+  <si>
+    <t>4cfc8be1-19ee-4685-bfb0-f793bd8db5d3</t>
+  </si>
+  <si>
+    <t>e606e963-3d68-4e52-91bd-172b28100c3b</t>
+  </si>
+  <si>
+    <t>520be2ef-4a9d-4fcf-9e88-82917c39c851</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5003,13 +5467,31 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF19191C"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -5039,7 +5521,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -5050,6 +5532,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="22" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="22" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5351,11 +5842,3563 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C8917CF-C27E-490B-8B89-4407CFDFA5CD}">
+  <dimension ref="A1:E67"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1647</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1648</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1649</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>405135394</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1651</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1652</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1653</v>
+      </c>
+      <c r="E2" s="6" t="str">
+        <f t="shared" ref="E2:E65" si="0">""&amp;IF(LEN(A2)=10,0&amp;A2,A2)</f>
+        <v>405135394</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>405461361</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1654</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1652</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1655</v>
+      </c>
+      <c r="E3" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>405461361</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>61007007408</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1656</v>
+      </c>
+      <c r="C4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1657</v>
+      </c>
+      <c r="E4" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>61007007408</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>445612864</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1658</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1652</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1669</v>
+      </c>
+      <c r="E5" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>445612864</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>31001054268</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1659</v>
+      </c>
+      <c r="C6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1779</v>
+      </c>
+      <c r="E6" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>31001054268</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1660</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1661</v>
+      </c>
+      <c r="C7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1662</v>
+      </c>
+      <c r="E7" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>C01492631</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>405429996</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1663</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1652</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1664</v>
+      </c>
+      <c r="E8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>405429996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1461</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1665</v>
+      </c>
+      <c r="C9" t="s">
+        <v>333</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1666</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>1780</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>441486517</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1667</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1652</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1668</v>
+      </c>
+      <c r="E10" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>441486517</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1461</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1658</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1652</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1669</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>1670</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1030048584</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1671</v>
+      </c>
+      <c r="C12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1672</v>
+      </c>
+      <c r="E12" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>01030048584</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>404760745</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1673</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1652</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1674</v>
+      </c>
+      <c r="E13" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>404760745</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>19001005737</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1675</v>
+      </c>
+      <c r="C14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1676</v>
+      </c>
+      <c r="E14" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>19001005737</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>61005000077</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1677</v>
+      </c>
+      <c r="C15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1678</v>
+      </c>
+      <c r="E15" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>61005000077</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>18001048942</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1679</v>
+      </c>
+      <c r="C16" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1680</v>
+      </c>
+      <c r="E16" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>18001048942</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>445500066</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1681</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1652</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1682</v>
+      </c>
+      <c r="E17" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>445500066</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>400340323</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1683</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1652</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1684</v>
+      </c>
+      <c r="E18" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>400340323</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>417875419</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1685</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1652</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1686</v>
+      </c>
+      <c r="E19" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>417875419</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>405753929</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1687</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1652</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1688</v>
+      </c>
+      <c r="E20" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>405753929</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>404387855</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1689</v>
+      </c>
+      <c r="C21" t="s">
+        <v>382</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1778</v>
+      </c>
+      <c r="E21" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>404387855</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1030003511</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1690</v>
+      </c>
+      <c r="C22" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1691</v>
+      </c>
+      <c r="E22" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>01030003511</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>405030504</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1692</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1652</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1693</v>
+      </c>
+      <c r="E23" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>405030504</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1024064734</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1694</v>
+      </c>
+      <c r="C24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1695</v>
+      </c>
+      <c r="E24" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>01024064734</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>48001007247</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1696</v>
+      </c>
+      <c r="C25" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1697</v>
+      </c>
+      <c r="E25" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>48001007247</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>62004003487</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1698</v>
+      </c>
+      <c r="C26" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1699</v>
+      </c>
+      <c r="E26" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>62004003487</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>62004003484</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1700</v>
+      </c>
+      <c r="C27" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1701</v>
+      </c>
+      <c r="E27" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>62004003484</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>13001067982</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1702</v>
+      </c>
+      <c r="C28" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1703</v>
+      </c>
+      <c r="E28" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>13001067982</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>9701030604</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1704</v>
+      </c>
+      <c r="C29" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1705</v>
+      </c>
+      <c r="E29" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>09701030604</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>30001010161</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1706</v>
+      </c>
+      <c r="C30" t="s">
+        <v>55</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1707</v>
+      </c>
+      <c r="E30" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>30001010161</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>1461</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1708</v>
+      </c>
+      <c r="C31" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" t="s">
+        <v>1709</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>1780</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>205273498</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1710</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1652</v>
+      </c>
+      <c r="D32" t="s">
+        <v>1711</v>
+      </c>
+      <c r="E32" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>205273498</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>443122871</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1712</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1652</v>
+      </c>
+      <c r="D33" t="s">
+        <v>1713</v>
+      </c>
+      <c r="E33" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>443122871</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>440893856</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1652</v>
+      </c>
+      <c r="D34" t="s">
+        <v>1715</v>
+      </c>
+      <c r="E34" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>440893856</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>1002016532</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1716</v>
+      </c>
+      <c r="C35" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" t="s">
+        <v>1717</v>
+      </c>
+      <c r="E35" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>01002016532</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>404742490</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1718</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1652</v>
+      </c>
+      <c r="D36" t="s">
+        <v>1719</v>
+      </c>
+      <c r="E36" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>404742490</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>61009020971</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1720</v>
+      </c>
+      <c r="C37" t="s">
+        <v>55</v>
+      </c>
+      <c r="D37" t="s">
+        <v>1721</v>
+      </c>
+      <c r="E37" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>61009020971</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1027043092</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1722</v>
+      </c>
+      <c r="C38" t="s">
+        <v>63</v>
+      </c>
+      <c r="D38" t="s">
+        <v>1723</v>
+      </c>
+      <c r="E38" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>01027043092</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>29001002303</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1724</v>
+      </c>
+      <c r="C39" t="s">
+        <v>63</v>
+      </c>
+      <c r="D39" t="s">
+        <v>1725</v>
+      </c>
+      <c r="E39" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>29001002303</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>404512737</v>
+      </c>
+      <c r="B40" t="s">
+        <v>1726</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1652</v>
+      </c>
+      <c r="D40" t="s">
+        <v>1727</v>
+      </c>
+      <c r="E40" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>404512737</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>1027057218</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1728</v>
+      </c>
+      <c r="C41" t="s">
+        <v>55</v>
+      </c>
+      <c r="D41" t="s">
+        <v>1729</v>
+      </c>
+      <c r="E41" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>01027057218</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>13001016058</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1730</v>
+      </c>
+      <c r="C42" t="s">
+        <v>55</v>
+      </c>
+      <c r="D42" t="s">
+        <v>1731</v>
+      </c>
+      <c r="E42" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>13001016058</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>38001039690</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1732</v>
+      </c>
+      <c r="C43" t="s">
+        <v>55</v>
+      </c>
+      <c r="D43" t="s">
+        <v>1733</v>
+      </c>
+      <c r="E43" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>38001039690</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>1027065735</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1734</v>
+      </c>
+      <c r="C44" t="s">
+        <v>55</v>
+      </c>
+      <c r="D44" t="s">
+        <v>1735</v>
+      </c>
+      <c r="E44" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>01027065735</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>1033004067</v>
+      </c>
+      <c r="B45" t="s">
+        <v>1736</v>
+      </c>
+      <c r="C45" t="s">
+        <v>55</v>
+      </c>
+      <c r="D45" t="s">
+        <v>1737</v>
+      </c>
+      <c r="E45" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>01033004067</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>400325457</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1738</v>
+      </c>
+      <c r="C46" t="s">
+        <v>1652</v>
+      </c>
+      <c r="D46" t="s">
+        <v>1739</v>
+      </c>
+      <c r="E46" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>400325457</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>1461</v>
+      </c>
+      <c r="B47" t="s">
+        <v>1740</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1652</v>
+      </c>
+      <c r="D47" t="s">
+        <v>1741</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>1742</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>1003015236</v>
+      </c>
+      <c r="B48" t="s">
+        <v>1743</v>
+      </c>
+      <c r="C48" t="s">
+        <v>55</v>
+      </c>
+      <c r="D48" t="s">
+        <v>1744</v>
+      </c>
+      <c r="E48" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>01003015236</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>4001003770</v>
+      </c>
+      <c r="B49" t="s">
+        <v>1745</v>
+      </c>
+      <c r="C49" t="s">
+        <v>63</v>
+      </c>
+      <c r="D49" t="s">
+        <v>1787</v>
+      </c>
+      <c r="E49" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>04001003770</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>1019082778</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1746</v>
+      </c>
+      <c r="C50" t="s">
+        <v>63</v>
+      </c>
+      <c r="D50" t="s">
+        <v>1747</v>
+      </c>
+      <c r="E50" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>01019082778</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>1461</v>
+      </c>
+      <c r="B51" t="s">
+        <v>1748</v>
+      </c>
+      <c r="C51" t="s">
+        <v>1652</v>
+      </c>
+      <c r="D51" t="s">
+        <v>1749</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>1750</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>211404531</v>
+      </c>
+      <c r="B52" t="s">
+        <v>1751</v>
+      </c>
+      <c r="C52" t="s">
+        <v>1652</v>
+      </c>
+      <c r="D52" t="s">
+        <v>1752</v>
+      </c>
+      <c r="E52" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>211404531</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>426558325</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1753</v>
+      </c>
+      <c r="C53" t="s">
+        <v>1652</v>
+      </c>
+      <c r="D53" t="s">
+        <v>1754</v>
+      </c>
+      <c r="E53" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>426558325</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>1461</v>
+      </c>
+      <c r="B54" t="s">
+        <v>1755</v>
+      </c>
+      <c r="C54" t="s">
+        <v>1652</v>
+      </c>
+      <c r="D54" t="s">
+        <v>1756</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>1757</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>404380629</v>
+      </c>
+      <c r="B55" t="s">
+        <v>1758</v>
+      </c>
+      <c r="C55" t="s">
+        <v>1652</v>
+      </c>
+      <c r="D55" t="s">
+        <v>1783</v>
+      </c>
+      <c r="E55" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>404380629</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>405753929</v>
+      </c>
+      <c r="B56" t="s">
+        <v>1687</v>
+      </c>
+      <c r="C56" t="s">
+        <v>1652</v>
+      </c>
+      <c r="D56" t="s">
+        <v>1688</v>
+      </c>
+      <c r="E56" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>405753929</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>345757772</v>
+      </c>
+      <c r="B57" t="s">
+        <v>1759</v>
+      </c>
+      <c r="C57" t="s">
+        <v>63</v>
+      </c>
+      <c r="D57" t="s">
+        <v>1760</v>
+      </c>
+      <c r="E57" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>345757772</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>1092003392</v>
+      </c>
+      <c r="B58" t="s">
+        <v>1761</v>
+      </c>
+      <c r="C58" t="s">
+        <v>55</v>
+      </c>
+      <c r="D58" t="s">
+        <v>1762</v>
+      </c>
+      <c r="E58" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>01092003392</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>443122871</v>
+      </c>
+      <c r="B59" t="s">
+        <v>1712</v>
+      </c>
+      <c r="C59" t="s">
+        <v>1652</v>
+      </c>
+      <c r="D59" t="s">
+        <v>1713</v>
+      </c>
+      <c r="E59" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>443122871</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>10610088510</v>
+      </c>
+      <c r="B60" t="s">
+        <v>1763</v>
+      </c>
+      <c r="C60" t="s">
+        <v>55</v>
+      </c>
+      <c r="D60" t="s">
+        <v>1764</v>
+      </c>
+      <c r="E60" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>10610088510</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>445598185</v>
+      </c>
+      <c r="B61" t="s">
+        <v>1765</v>
+      </c>
+      <c r="C61" t="s">
+        <v>1652</v>
+      </c>
+      <c r="D61" t="s">
+        <v>1766</v>
+      </c>
+      <c r="E61" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>445598185</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>211349762</v>
+      </c>
+      <c r="B62" t="s">
+        <v>1767</v>
+      </c>
+      <c r="C62" t="s">
+        <v>1768</v>
+      </c>
+      <c r="D62" t="s">
+        <v>1769</v>
+      </c>
+      <c r="E62" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>211349762</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>231289593</v>
+      </c>
+      <c r="B63" t="s">
+        <v>1770</v>
+      </c>
+      <c r="C63" t="s">
+        <v>1652</v>
+      </c>
+      <c r="D63" t="s">
+        <v>1784</v>
+      </c>
+      <c r="E63" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>231289593</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>405665285</v>
+      </c>
+      <c r="B64" t="s">
+        <v>1771</v>
+      </c>
+      <c r="C64" t="s">
+        <v>1652</v>
+      </c>
+      <c r="D64" t="s">
+        <v>1785</v>
+      </c>
+      <c r="E64" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>405665285</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>205064446</v>
+      </c>
+      <c r="B65" t="s">
+        <v>1772</v>
+      </c>
+      <c r="C65" t="s">
+        <v>1652</v>
+      </c>
+      <c r="D65" t="s">
+        <v>1773</v>
+      </c>
+      <c r="E65" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>205064446</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>57001010449</v>
+      </c>
+      <c r="B66" t="s">
+        <v>1774</v>
+      </c>
+      <c r="C66" t="s">
+        <v>55</v>
+      </c>
+      <c r="D66" t="s">
+        <v>1775</v>
+      </c>
+      <c r="E66" s="6" t="str">
+        <f t="shared" ref="E66" si="1">""&amp;IF(LEN(A66)=10,0&amp;A66,A66)</f>
+        <v>57001010449</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>445721595</v>
+      </c>
+      <c r="B67" t="s">
+        <v>1776</v>
+      </c>
+      <c r="C67" t="s">
+        <v>1652</v>
+      </c>
+      <c r="D67" t="s">
+        <v>1777</v>
+      </c>
+      <c r="E67" s="6" t="str">
+        <f>""&amp;IF(LEN(A67)=10,0&amp;A67,A67)</f>
+        <v>445721595</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:E67" xr:uid="{0C8917CF-C27E-490B-8B89-4407CFDFA5CD}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E550398-190A-4F15-BF25-77B6E32729EB}">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:Z277"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="S72" sqref="S72"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="80.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="21" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9"/>
+      <c r="B2" s="10" t="str" cm="1">
+        <f t="array" ref="B2:B67">Sheet3!D2:D67</f>
+        <v>გეა ნოვა</v>
+      </c>
+      <c r="C2" s="11" t="str" cm="1">
+        <f t="array" ref="C2:C67">Sheet3!E2:E67</f>
+        <v>405135394</v>
+      </c>
+      <c r="D2" s="12"/>
+      <c r="E2" s="10" t="str" cm="1">
+        <f t="array" ref="E2:E67">Sheet3!C2:C67</f>
+        <v xml:space="preserve">შპს </v>
+      </c>
+      <c r="K2" s="10" t="str" cm="1">
+        <f t="array" ref="K2:K67">Sheet3!B2:B67</f>
+        <v>GE96BG0000000730563700GEL</v>
+      </c>
+      <c r="S2" s="10" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T2" s="10" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="10" t="str">
+        <v>ჯი თი სი რენთ</v>
+      </c>
+      <c r="C3" s="10" t="str">
+        <v>405461361</v>
+      </c>
+      <c r="D3" s="12"/>
+      <c r="E3" s="10" t="str">
+        <v xml:space="preserve">შპს </v>
+      </c>
+      <c r="K3" s="10" t="str">
+        <v>GE24TB7236936020100010</v>
+      </c>
+      <c r="S3" s="10" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T3" s="10" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" t="str">
+        <v>ტოროსიანი მარინა</v>
+      </c>
+      <c r="C4" t="str">
+        <v>61007007408</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" t="str">
+        <v>ფიზ. პირი</v>
+      </c>
+      <c r="F4" t="s">
+        <v>84</v>
+      </c>
+      <c r="K4" t="str">
+        <v>GE84BG0000000100756011GEL</v>
+      </c>
+      <c r="S4" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T4" t="s">
+        <v>1786</v>
+      </c>
+      <c r="W4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="B5" s="10" t="str">
+        <v>აი ეს ბი ეიჩ</v>
+      </c>
+      <c r="C5" s="10" t="str">
+        <v>445612864</v>
+      </c>
+      <c r="D5" s="12"/>
+      <c r="E5" s="10" t="str">
+        <v xml:space="preserve">შპს </v>
+      </c>
+      <c r="K5" s="10" t="str">
+        <v>GE05BS0000000010936920</v>
+      </c>
+      <c r="S5" s="10" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T5" s="10" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
+      <c r="B6" s="10" t="str">
+        <v>თორნიკე პაპიაშვილი</v>
+      </c>
+      <c r="C6" s="10" t="str">
+        <v>31001054268</v>
+      </c>
+      <c r="D6" s="12"/>
+      <c r="E6" s="10" t="str">
+        <v>ინდ. მეწარმე</v>
+      </c>
+      <c r="K6" s="10" t="str">
+        <v>GE26BG0000000528006165GEL</v>
+      </c>
+      <c r="S6" s="10" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T6" s="10" t="s">
+        <v>1786</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" t="str">
+        <v>აანდიყევ ალასგარ</v>
+      </c>
+      <c r="C7" t="str">
+        <v>C01492631</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" t="str">
+        <v>ფიზ. პირი</v>
+      </c>
+      <c r="F7" t="s">
+        <v>54</v>
+      </c>
+      <c r="K7" t="str">
+        <v>GE92BG0000000609672187GEL</v>
+      </c>
+      <c r="S7" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T7" t="s">
+        <v>1786</v>
+      </c>
+      <c r="W7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="10" t="str">
+        <v>ნიკოლას</v>
+      </c>
+      <c r="C8" s="10" t="str">
+        <v>405429996</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="10" t="str">
+        <v xml:space="preserve">შპს </v>
+      </c>
+      <c r="K8" s="10" t="str">
+        <v>GE07BG0000000523441105GEL</v>
+      </c>
+      <c r="S8" s="10" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T8" s="10" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" t="str">
+        <v>Hidral</v>
+      </c>
+      <c r="C9" t="str">
+        <v>61007007408</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" t="str">
+        <v>უცხოური საწარმო</v>
+      </c>
+      <c r="K9" t="str">
+        <v>ES7500815094800001135224</v>
+      </c>
+      <c r="S9" t="s">
+        <v>1792</v>
+      </c>
+      <c r="T9" s="8" t="s">
+        <v>1788</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
+      <c r="B10" s="10" t="str">
+        <v>ტეკი</v>
+      </c>
+      <c r="C10" s="10" t="str">
+        <v>441486517</v>
+      </c>
+      <c r="D10" s="12"/>
+      <c r="E10" s="10" t="str">
+        <v xml:space="preserve">შპს </v>
+      </c>
+      <c r="K10" s="10" t="str">
+        <v>GE84BG0000000161360738GEL</v>
+      </c>
+      <c r="S10" s="10" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T10" s="10" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+      <c r="B11" s="10" t="str">
+        <v>აი ეს ბი ეიჩ</v>
+      </c>
+      <c r="C11" s="10" t="str">
+        <v>445612864</v>
+      </c>
+      <c r="D11" s="12"/>
+      <c r="E11" s="10" t="str">
+        <v xml:space="preserve">შპს </v>
+      </c>
+      <c r="K11" s="10" t="str">
+        <v>GE05BS0000000010936920</v>
+      </c>
+      <c r="S11" s="10" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T11" s="10" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" t="str">
+        <v>მორჩილაძე მარიანა</v>
+      </c>
+      <c r="C12" t="str">
+        <v>01030048584</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="E12" t="str">
+        <v>ფიზ. პირი</v>
+      </c>
+      <c r="F12" t="s">
+        <v>84</v>
+      </c>
+      <c r="K12" t="str">
+        <v>GE80BG0000000498659686GEL</v>
+      </c>
+      <c r="S12" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T12" t="s">
+        <v>1786</v>
+      </c>
+      <c r="W12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
+      <c r="B13" s="10" t="str">
+        <v>რობირენტ.ჯი</v>
+      </c>
+      <c r="C13" s="10" t="str">
+        <v>404760745</v>
+      </c>
+      <c r="D13" s="12"/>
+      <c r="E13" s="10" t="str">
+        <v xml:space="preserve">შპს </v>
+      </c>
+      <c r="K13" s="10" t="str">
+        <v>GE52BG0000000606293330GEL</v>
+      </c>
+      <c r="S13" s="10" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T13" s="10" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" t="str">
+        <v>იზორია გიორგი</v>
+      </c>
+      <c r="C14" t="str">
+        <v>19001005737</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" t="str">
+        <v>ფიზ. პირი</v>
+      </c>
+      <c r="F14" t="s">
+        <v>54</v>
+      </c>
+      <c r="K14" t="str">
+        <v>GE82BG0000000541362251GEL</v>
+      </c>
+      <c r="S14" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T14" t="s">
+        <v>1786</v>
+      </c>
+      <c r="W14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" t="str">
+        <v>ტარიელაძე თეიმურაზ</v>
+      </c>
+      <c r="C15" t="str">
+        <v>61005000077</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15" t="str">
+        <v>ფიზ. პირი</v>
+      </c>
+      <c r="F15" t="s">
+        <v>54</v>
+      </c>
+      <c r="K15" t="str">
+        <v>GE54BG0000000162677471GEL</v>
+      </c>
+      <c r="S15" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T15" t="s">
+        <v>1786</v>
+      </c>
+      <c r="W15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="9"/>
+      <c r="B16" s="10" t="str">
+        <v>ამირან წაქაძე</v>
+      </c>
+      <c r="C16" s="10" t="str">
+        <v>18001048942</v>
+      </c>
+      <c r="D16" s="12"/>
+      <c r="E16" s="10" t="str">
+        <v>ინდ. მეწარმე</v>
+      </c>
+      <c r="K16" s="10" t="str">
+        <v>GE13BG0000000534065989GEL</v>
+      </c>
+      <c r="S16" s="10" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T16" s="10" t="s">
+        <v>1786</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="9"/>
+      <c r="B17" s="10" t="str">
+        <v>სტატუსი</v>
+      </c>
+      <c r="C17" s="10" t="str">
+        <v>445500066</v>
+      </c>
+      <c r="D17" s="12"/>
+      <c r="E17" s="10" t="str">
+        <v xml:space="preserve">შპს </v>
+      </c>
+      <c r="K17" s="10" t="str">
+        <v>GE83BG0000000548350598GEL</v>
+      </c>
+      <c r="S17" s="10" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T17" s="10" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="9"/>
+      <c r="B18" s="10" t="str">
+        <v>უნივერსალური ნათება</v>
+      </c>
+      <c r="C18" s="10" t="str">
+        <v>400340323</v>
+      </c>
+      <c r="D18" s="12"/>
+      <c r="E18" s="10" t="str">
+        <v xml:space="preserve">შპს </v>
+      </c>
+      <c r="K18" s="10" t="str">
+        <v>GE93BG0000000538027969GEL</v>
+      </c>
+      <c r="S18" s="10" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T18" s="10" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="9"/>
+      <c r="B19" s="10" t="str">
+        <v>ლაცა 2009</v>
+      </c>
+      <c r="C19" s="10" t="str">
+        <v>417875419</v>
+      </c>
+      <c r="D19" s="12"/>
+      <c r="E19" s="10" t="str">
+        <v xml:space="preserve">შპს </v>
+      </c>
+      <c r="K19" s="10" t="str">
+        <v>GE02BG0000000622833700GEL</v>
+      </c>
+      <c r="S19" s="10" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T19" s="10" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="9"/>
+      <c r="B20" s="10" t="str">
+        <v>ჩექ ქარ ჯეორჯია</v>
+      </c>
+      <c r="C20" s="10" t="str">
+        <v>405753929</v>
+      </c>
+      <c r="D20" s="12"/>
+      <c r="E20" s="10" t="str">
+        <v xml:space="preserve">შპს </v>
+      </c>
+      <c r="K20" s="10" t="str">
+        <v>GE63BG0000000606154034GEL</v>
+      </c>
+      <c r="S20" s="10" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T20" s="10" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" t="str">
+        <v>საქართველოს მცირე და საშუალო საწარმოთა ასოციაცია</v>
+      </c>
+      <c r="C21" t="str">
+        <v>404387855</v>
+      </c>
+      <c r="D21" s="5"/>
+      <c r="E21" t="str">
+        <v>არასამეწარმეო (არაკომერციული) იურიდიული პირი</v>
+      </c>
+      <c r="K21" t="str">
+        <v>GE52BG0000000594459718GEL</v>
+      </c>
+      <c r="S21" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T21" s="8" t="s">
+        <v>1789</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" t="str">
+        <v>ირემაშვილი აკაკი</v>
+      </c>
+      <c r="C22" t="str">
+        <v>01030003511</v>
+      </c>
+      <c r="D22" s="5"/>
+      <c r="E22" t="str">
+        <v>ფიზ. პირი</v>
+      </c>
+      <c r="F22" t="s">
+        <v>54</v>
+      </c>
+      <c r="K22" t="str">
+        <v>GE38BG0000000101462223GEL</v>
+      </c>
+      <c r="S22" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T22" t="s">
+        <v>1786</v>
+      </c>
+      <c r="W22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="9"/>
+      <c r="B23" s="10" t="str">
+        <v>თრეიდერი</v>
+      </c>
+      <c r="C23" s="10" t="str">
+        <v>405030504</v>
+      </c>
+      <c r="D23" s="12"/>
+      <c r="E23" s="10" t="str">
+        <v xml:space="preserve">შპს </v>
+      </c>
+      <c r="K23" s="10" t="str">
+        <v>GE26TB7212436050100001</v>
+      </c>
+      <c r="S23" s="10" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T23" s="10" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" t="str">
+        <v>მჟავია დარეჯან</v>
+      </c>
+      <c r="C24" t="str">
+        <v>01024064734</v>
+      </c>
+      <c r="D24" s="5"/>
+      <c r="E24" t="str">
+        <v>ფიზ. პირი</v>
+      </c>
+      <c r="F24" t="s">
+        <v>84</v>
+      </c>
+      <c r="K24" t="str">
+        <v>GE31BG0000000162627833GEL</v>
+      </c>
+      <c r="S24" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T24" t="s">
+        <v>1786</v>
+      </c>
+      <c r="W24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" t="str">
+        <v>ქებურია ნიკა</v>
+      </c>
+      <c r="C25" t="str">
+        <v>48001007247</v>
+      </c>
+      <c r="D25" s="5"/>
+      <c r="E25" t="str">
+        <v>ფიზ. პირი</v>
+      </c>
+      <c r="F25" t="s">
+        <v>54</v>
+      </c>
+      <c r="K25" t="str">
+        <v>GE41BG0000000346051064GEL</v>
+      </c>
+      <c r="S25" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T25" t="s">
+        <v>1786</v>
+      </c>
+      <c r="W25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" t="str">
+        <v>კორთხონჯია დავით</v>
+      </c>
+      <c r="C26" t="str">
+        <v>62004003487</v>
+      </c>
+      <c r="D26" s="5"/>
+      <c r="E26" t="str">
+        <v>ფიზ. პირი</v>
+      </c>
+      <c r="F26" t="s">
+        <v>54</v>
+      </c>
+      <c r="K26" t="str">
+        <v>GE52BG0000000808306500GEL</v>
+      </c>
+      <c r="S26" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T26" t="s">
+        <v>1786</v>
+      </c>
+      <c r="W26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" t="str">
+        <v>კორთხონჯია ზურაბ</v>
+      </c>
+      <c r="C27" t="str">
+        <v>62004003484</v>
+      </c>
+      <c r="D27" s="5"/>
+      <c r="E27" t="str">
+        <v>ფიზ. პირი</v>
+      </c>
+      <c r="F27" t="s">
+        <v>54</v>
+      </c>
+      <c r="K27" t="str">
+        <v>GE37BG0000000131254142GEL</v>
+      </c>
+      <c r="S27" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T27" t="s">
+        <v>1786</v>
+      </c>
+      <c r="W27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" t="str">
+        <v>მამულაშვილი შალვა</v>
+      </c>
+      <c r="C28" t="str">
+        <v>13001067982</v>
+      </c>
+      <c r="D28" s="5"/>
+      <c r="E28" t="str">
+        <v>ფიზ. პირი</v>
+      </c>
+      <c r="F28" t="s">
+        <v>54</v>
+      </c>
+      <c r="K28" t="str">
+        <v>GE56BG0000000366036092GEL</v>
+      </c>
+      <c r="S28" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T28" t="s">
+        <v>1786</v>
+      </c>
+      <c r="W28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" t="str">
+        <v>ფუტკარაძე გივი</v>
+      </c>
+      <c r="C29" t="str">
+        <v>09701030604</v>
+      </c>
+      <c r="D29" s="5"/>
+      <c r="E29" t="str">
+        <v>ფიზ. პირი</v>
+      </c>
+      <c r="F29" t="s">
+        <v>54</v>
+      </c>
+      <c r="K29" t="str">
+        <v>GE52BG0000000101309875GEL</v>
+      </c>
+      <c r="S29" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T29" t="s">
+        <v>1786</v>
+      </c>
+      <c r="W29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" t="str">
+        <v>შერვაშიძე ერეკლე</v>
+      </c>
+      <c r="C30" t="str">
+        <v>30001010161</v>
+      </c>
+      <c r="D30" s="5"/>
+      <c r="E30" t="str">
+        <v>ფიზ. პირი</v>
+      </c>
+      <c r="F30" t="s">
+        <v>54</v>
+      </c>
+      <c r="K30" t="str">
+        <v>GE36BG0000000584703164GEL</v>
+      </c>
+      <c r="S30" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T30" t="s">
+        <v>1786</v>
+      </c>
+      <c r="W30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" t="str">
+        <v>მარინა ტოროსიანი</v>
+      </c>
+      <c r="C31" t="str">
+        <v>61007007408</v>
+      </c>
+      <c r="D31" s="5"/>
+      <c r="E31" t="str">
+        <v>ფიზ. პირი</v>
+      </c>
+      <c r="F31" t="s">
+        <v>84</v>
+      </c>
+      <c r="K31" t="str">
+        <v>GE29TB7598345064300061</v>
+      </c>
+      <c r="S31" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T31" t="s">
+        <v>1786</v>
+      </c>
+      <c r="W31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="9"/>
+      <c r="B32" s="10" t="str">
+        <v>არბო 2009</v>
+      </c>
+      <c r="C32" s="10" t="str">
+        <v>205273498</v>
+      </c>
+      <c r="D32" s="12"/>
+      <c r="E32" s="10" t="str">
+        <v xml:space="preserve">შპს </v>
+      </c>
+      <c r="K32" s="10" t="str">
+        <v>GE97TB7713036060100001</v>
+      </c>
+      <c r="S32" s="10" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T32" s="10" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="9"/>
+      <c r="B33" s="10" t="str">
+        <v>ჯე ფიტტინგ</v>
+      </c>
+      <c r="C33" s="10" t="str">
+        <v>443122871</v>
+      </c>
+      <c r="D33" s="12"/>
+      <c r="E33" s="10" t="str">
+        <v xml:space="preserve">შპს </v>
+      </c>
+      <c r="K33" s="10" t="str">
+        <v>GE08BG0000000366075562GEL</v>
+      </c>
+      <c r="S33" s="10" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T33" s="10" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="9"/>
+      <c r="B34" s="10" t="str">
+        <v>ფართი შოპ ჯი</v>
+      </c>
+      <c r="C34" s="10" t="str">
+        <v>440893856</v>
+      </c>
+      <c r="D34" s="12"/>
+      <c r="E34" s="10" t="str">
+        <v xml:space="preserve">შპს </v>
+      </c>
+      <c r="K34" s="10" t="str">
+        <v>GE60BG0000000537555494GEL</v>
+      </c>
+      <c r="S34" s="10" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T34" s="10" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="B35" t="str">
+        <v>ჟანა ოგანეზოვი</v>
+      </c>
+      <c r="C35" t="str">
+        <v>01002016532</v>
+      </c>
+      <c r="D35" s="5"/>
+      <c r="E35" t="str">
+        <v>ფიზ. პირი</v>
+      </c>
+      <c r="F35" t="s">
+        <v>84</v>
+      </c>
+      <c r="K35" t="str">
+        <v>GE85TB7151545061100023</v>
+      </c>
+      <c r="S35" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T35" t="s">
+        <v>1786</v>
+      </c>
+      <c r="W35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="9"/>
+      <c r="B36" s="10" t="str">
+        <v>იში7788</v>
+      </c>
+      <c r="C36" s="10" t="str">
+        <v>404742490</v>
+      </c>
+      <c r="D36" s="12"/>
+      <c r="E36" s="10" t="str">
+        <v xml:space="preserve">შპს </v>
+      </c>
+      <c r="K36" s="10" t="str">
+        <v>GE05TB7886536080100008</v>
+      </c>
+      <c r="S36" s="10" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T36" s="10" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2"/>
+      <c r="B37" t="str">
+        <v>ცეცხლაძე როინ</v>
+      </c>
+      <c r="C37" t="str">
+        <v>61009020971</v>
+      </c>
+      <c r="D37" s="5"/>
+      <c r="E37" t="str">
+        <v>ფიზ. პირი</v>
+      </c>
+      <c r="F37" t="s">
+        <v>54</v>
+      </c>
+      <c r="K37" t="str">
+        <v>GE21BG0000000759214000GEL</v>
+      </c>
+      <c r="S37" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T37" t="s">
+        <v>1786</v>
+      </c>
+      <c r="W37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="9"/>
+      <c r="B38" s="10" t="str">
+        <v>მურმან გეგია</v>
+      </c>
+      <c r="C38" s="10" t="str">
+        <v>01027043092</v>
+      </c>
+      <c r="D38" s="12"/>
+      <c r="E38" s="10" t="str">
+        <v>ინდ. მეწარმე</v>
+      </c>
+      <c r="K38" s="10" t="str">
+        <v>GE95BG0000000695964400GEL</v>
+      </c>
+      <c r="S38" s="10" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T38" s="10" t="s">
+        <v>1786</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="9"/>
+      <c r="B39" s="10" t="str">
+        <v>ლარისა ფონიავა</v>
+      </c>
+      <c r="C39" s="10" t="str">
+        <v>29001002303</v>
+      </c>
+      <c r="D39" s="12"/>
+      <c r="E39" s="10" t="str">
+        <v>ინდ. მეწარმე</v>
+      </c>
+      <c r="K39" s="10" t="str">
+        <v>GE57BG0000000215070900GEL</v>
+      </c>
+      <c r="S39" s="10" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T39" s="10" t="s">
+        <v>1786</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="9"/>
+      <c r="B40" s="10" t="str">
+        <v xml:space="preserve"> ოაგრუპ</v>
+      </c>
+      <c r="C40" s="10" t="str">
+        <v>404512737</v>
+      </c>
+      <c r="D40" s="12"/>
+      <c r="E40" s="10" t="str">
+        <v xml:space="preserve">შპს </v>
+      </c>
+      <c r="K40" s="10" t="str">
+        <v>GE23TB7185636080100003</v>
+      </c>
+      <c r="S40" s="10" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T40" s="10" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="2"/>
+      <c r="B41" t="str">
+        <v>ოთარაშვილი ალექსეი</v>
+      </c>
+      <c r="C41" t="str">
+        <v>01027057218</v>
+      </c>
+      <c r="D41" s="5"/>
+      <c r="E41" t="str">
+        <v>ფიზ. პირი</v>
+      </c>
+      <c r="F41" t="s">
+        <v>54</v>
+      </c>
+      <c r="K41" t="str">
+        <v>GE84BG0000000103359782GEL</v>
+      </c>
+      <c r="S41" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T41" t="s">
+        <v>1786</v>
+      </c>
+      <c r="W41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2"/>
+      <c r="B42" t="str">
+        <v>კვეზერელი ნიკოლოზ</v>
+      </c>
+      <c r="C42" t="str">
+        <v>13001016058</v>
+      </c>
+      <c r="E42" t="str">
+        <v>ფიზ. პირი</v>
+      </c>
+      <c r="F42" t="s">
+        <v>54</v>
+      </c>
+      <c r="K42" t="str">
+        <v>GE08BG0000000312837500GEL</v>
+      </c>
+      <c r="S42" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T42" t="s">
+        <v>1786</v>
+      </c>
+      <c r="W42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2"/>
+      <c r="B43" t="str">
+        <v>სოფიკო ხომასურიძე</v>
+      </c>
+      <c r="C43" t="str">
+        <v>38001039690</v>
+      </c>
+      <c r="E43" t="str">
+        <v>ფიზ. პირი</v>
+      </c>
+      <c r="F43" t="s">
+        <v>84</v>
+      </c>
+      <c r="K43" t="str">
+        <v>GE87LB0211117682002000</v>
+      </c>
+      <c r="S43" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T43" t="s">
+        <v>1786</v>
+      </c>
+      <c r="W43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2"/>
+      <c r="B44" t="str">
+        <v>მუკბანიანი ანა</v>
+      </c>
+      <c r="C44" t="str">
+        <v>01027065735</v>
+      </c>
+      <c r="E44" t="str">
+        <v>ფიზ. პირი</v>
+      </c>
+      <c r="F44" t="s">
+        <v>84</v>
+      </c>
+      <c r="K44" t="str">
+        <v>GE20BG0000000161924296GEL</v>
+      </c>
+      <c r="S44" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T44" t="s">
+        <v>1786</v>
+      </c>
+      <c r="W44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2"/>
+      <c r="B45" t="str">
+        <v>ბულბულაშვილი ნოდარი</v>
+      </c>
+      <c r="C45" t="str">
+        <v>01033004067</v>
+      </c>
+      <c r="E45" t="str">
+        <v>ფიზ. პირი</v>
+      </c>
+      <c r="F45" t="s">
+        <v>54</v>
+      </c>
+      <c r="K45" t="str">
+        <v>GE92BG0000000187220600GEL</v>
+      </c>
+      <c r="S45" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T45" t="s">
+        <v>1786</v>
+      </c>
+      <c r="W45" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="9"/>
+      <c r="B46" s="10" t="str">
+        <v>ნანოტეკ ფროდაქშენ</v>
+      </c>
+      <c r="C46" s="10" t="str">
+        <v>400325457</v>
+      </c>
+      <c r="E46" s="10" t="str">
+        <v xml:space="preserve">შპს </v>
+      </c>
+      <c r="K46" s="10" t="str">
+        <v>GE95TB7931136020100009</v>
+      </c>
+      <c r="S46" s="10" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T46" s="10" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="9"/>
+      <c r="B47" s="10" t="str">
+        <v>ბაგრო ჯორჯია</v>
+      </c>
+      <c r="C47" s="10" t="str">
+        <v>400438371</v>
+      </c>
+      <c r="E47" s="10" t="str">
+        <v xml:space="preserve">შპს </v>
+      </c>
+      <c r="K47" s="10" t="str">
+        <v>GE20TB7938836020100004</v>
+      </c>
+      <c r="S47" s="10" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T47" s="10" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="2"/>
+      <c r="B48" t="str">
+        <v>ბექაური ქეთევან</v>
+      </c>
+      <c r="C48" t="str">
+        <v>01003015236</v>
+      </c>
+      <c r="E48" t="str">
+        <v>ფიზ. პირი</v>
+      </c>
+      <c r="F48" t="s">
+        <v>84</v>
+      </c>
+      <c r="K48" t="str">
+        <v>GE94BG0000000654109500GEL</v>
+      </c>
+      <c r="S48" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T48" t="s">
+        <v>1786</v>
+      </c>
+      <c r="W48" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="9"/>
+      <c r="B49" s="10" t="str">
+        <v>ნიკოლოზ ოშხერელი</v>
+      </c>
+      <c r="C49" s="10" t="str">
+        <v>04001003770</v>
+      </c>
+      <c r="E49" s="10" t="str">
+        <v>ინდ. მეწარმე</v>
+      </c>
+      <c r="K49" s="10" t="str">
+        <v>GE32BG0000000541718947GEL</v>
+      </c>
+      <c r="S49" s="10" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T49" s="10" t="s">
+        <v>1786</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="9"/>
+      <c r="B50" s="10" t="str">
+        <v>ილია ცინცაძე</v>
+      </c>
+      <c r="C50" s="10" t="str">
+        <v>01019082778</v>
+      </c>
+      <c r="E50" s="10" t="str">
+        <v>ინდ. მეწარმე</v>
+      </c>
+      <c r="K50" s="10" t="str">
+        <v>GE37BG0000000610791684GEL</v>
+      </c>
+      <c r="S50" s="10" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T50" s="10" t="s">
+        <v>1786</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="9"/>
+      <c r="B51" s="10" t="str">
+        <v>ველლი ჯგუფი</v>
+      </c>
+      <c r="C51" s="10" t="str">
+        <v>429336621</v>
+      </c>
+      <c r="E51" s="10" t="str">
+        <v xml:space="preserve">შპს </v>
+      </c>
+      <c r="K51" s="10" t="str">
+        <v>GE50TB7080036060100002</v>
+      </c>
+      <c r="S51" s="10" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T51" s="10" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="9"/>
+      <c r="B52" s="10" t="str">
+        <v>სიდო</v>
+      </c>
+      <c r="C52" s="10" t="str">
+        <v>211404531</v>
+      </c>
+      <c r="E52" s="10" t="str">
+        <v xml:space="preserve">შპს </v>
+      </c>
+      <c r="K52" s="10" t="str">
+        <v>GE08PC0183600100015821</v>
+      </c>
+      <c r="S52" s="10" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T52" s="10" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="53" spans="1:23" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="9"/>
+      <c r="B53" s="10" t="str">
+        <v>ვერტა ელევატორი</v>
+      </c>
+      <c r="C53" s="10" t="str">
+        <v>426558325</v>
+      </c>
+      <c r="E53" s="10" t="str">
+        <v xml:space="preserve">შპს </v>
+      </c>
+      <c r="K53" s="10" t="str">
+        <v>GE32TB7372336080100012</v>
+      </c>
+      <c r="S53" s="10" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T53" s="10" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="54" spans="1:23" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="9"/>
+      <c r="B54" s="10" t="str">
+        <v>კოკოსილქ+</v>
+      </c>
+      <c r="C54" s="10" t="str">
+        <v>406320887</v>
+      </c>
+      <c r="E54" s="10" t="str">
+        <v xml:space="preserve">შპს </v>
+      </c>
+      <c r="K54" s="10" t="str">
+        <v>GE69TB7863336080100016</v>
+      </c>
+      <c r="S54" s="10" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T54" s="10" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="9"/>
+      <c r="B55" s="10" t="str">
+        <v>ნიუ მეტალ ჯორჯია</v>
+      </c>
+      <c r="C55" s="10" t="str">
+        <v>404380629</v>
+      </c>
+      <c r="E55" s="10" t="str">
+        <v xml:space="preserve">შპს </v>
+      </c>
+      <c r="K55" s="10" t="str">
+        <v>GE29TB3900000077517777</v>
+      </c>
+      <c r="S55" s="10" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T55" s="10" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="9"/>
+      <c r="B56" s="10" t="str">
+        <v>ჩექ ქარ ჯეორჯია</v>
+      </c>
+      <c r="C56" s="10" t="str">
+        <v>405753929</v>
+      </c>
+      <c r="E56" s="10" t="str">
+        <v xml:space="preserve">შპს </v>
+      </c>
+      <c r="K56" s="10" t="str">
+        <v>GE63BG0000000606154034GEL</v>
+      </c>
+      <c r="S56" s="10" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T56" s="10" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="57" spans="1:23" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="13"/>
+      <c r="B57" s="14" t="str">
+        <v>ვასილიი კაპლიევ</v>
+      </c>
+      <c r="C57" s="14" t="str">
+        <v>345757772</v>
+      </c>
+      <c r="E57" s="14" t="str">
+        <v>ინდ. მეწარმე</v>
+      </c>
+      <c r="K57" s="14" t="str">
+        <v>GE29TB7400836010100046</v>
+      </c>
+      <c r="S57" s="14" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T57" s="14" t="s">
+        <v>1786</v>
+      </c>
+    </row>
+    <row r="58" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="2"/>
+      <c r="B58" t="str">
+        <v>მამმადოვ როვშან</v>
+      </c>
+      <c r="C58" t="str">
+        <v>01092003392</v>
+      </c>
+      <c r="E58" t="str">
+        <v>ფიზ. პირი</v>
+      </c>
+      <c r="F58" t="s">
+        <v>54</v>
+      </c>
+      <c r="K58" t="str">
+        <v>GE73BG0000000279352900GEL</v>
+      </c>
+      <c r="S58" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T58" t="s">
+        <v>1786</v>
+      </c>
+      <c r="W58" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:23" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="9"/>
+      <c r="B59" s="10" t="str">
+        <v>ჯე ფიტტინგ</v>
+      </c>
+      <c r="C59" s="10" t="str">
+        <v>443122871</v>
+      </c>
+      <c r="E59" s="10" t="str">
+        <v xml:space="preserve">შპს </v>
+      </c>
+      <c r="K59" s="10" t="str">
+        <v>GE08BG0000000366075562GEL</v>
+      </c>
+      <c r="S59" s="10" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T59" s="10" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="60" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="2"/>
+      <c r="B60" t="str">
+        <v>ცანქალ მუამმერ</v>
+      </c>
+      <c r="C60" t="str">
+        <v>10610088510</v>
+      </c>
+      <c r="E60" t="str">
+        <v>ფიზ. პირი</v>
+      </c>
+      <c r="F60" t="s">
+        <v>54</v>
+      </c>
+      <c r="K60" t="str">
+        <v>GE53BG0000000545804791GEL</v>
+      </c>
+      <c r="S60" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T60" t="s">
+        <v>1786</v>
+      </c>
+      <c r="W60" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:23" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="9"/>
+      <c r="B61" s="10" t="str">
+        <v>უნიკალი</v>
+      </c>
+      <c r="C61" s="10" t="str">
+        <v>445598185</v>
+      </c>
+      <c r="E61" s="10" t="str">
+        <v xml:space="preserve">შპს </v>
+      </c>
+      <c r="K61" s="10" t="str">
+        <v>GE88BG0000000499033380GEL</v>
+      </c>
+      <c r="S61" s="10" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T61" s="10" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A62" s="2"/>
+      <c r="B62" t="str">
+        <v>EMBASSY OF ISLAMIC REPUBLIC OF IRAN</v>
+      </c>
+      <c r="C62" t="str">
+        <v>211349762</v>
+      </c>
+      <c r="E62" t="str">
+        <v>დიპლომატი</v>
+      </c>
+      <c r="K62" t="str">
+        <v>GE34TB0600000000609009</v>
+      </c>
+      <c r="S62" t="s">
+        <v>1791</v>
+      </c>
+      <c r="T62" s="8" t="s">
+        <v>1790</v>
+      </c>
+    </row>
+    <row r="63" spans="1:23" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="9"/>
+      <c r="B63" s="10" t="str">
+        <v>საერთაშორისო სავაჭრო ჯგუფი</v>
+      </c>
+      <c r="C63" s="10" t="str">
+        <v>231289593</v>
+      </c>
+      <c r="E63" s="10" t="str">
+        <v xml:space="preserve">შპს </v>
+      </c>
+      <c r="K63" s="10" t="str">
+        <v>GE11TB1930636080100002</v>
+      </c>
+      <c r="S63" s="10" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T63" s="10" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="64" spans="1:23" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="9"/>
+      <c r="B64" s="10" t="str">
+        <v>ოქტო არტჰაუსი</v>
+      </c>
+      <c r="C64" s="10" t="str">
+        <v>405665285</v>
+      </c>
+      <c r="E64" s="10" t="str">
+        <v xml:space="preserve">შპს </v>
+      </c>
+      <c r="K64" s="10" t="str">
+        <v>GE62TB7183936050100002</v>
+      </c>
+      <c r="S64" s="10" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T64" s="10" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="65" spans="1:23" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="9"/>
+      <c r="B65" s="10" t="str">
+        <v>საქსპეცტრანსი</v>
+      </c>
+      <c r="C65" s="10" t="str">
+        <v>205064446</v>
+      </c>
+      <c r="E65" s="10" t="str">
+        <v xml:space="preserve">შპს </v>
+      </c>
+      <c r="K65" s="10" t="str">
+        <v>GE92BG0000000545811849GEL</v>
+      </c>
+      <c r="S65" s="10" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T65" s="10" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="66" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="2"/>
+      <c r="B66" t="str">
+        <v>ხაჭაპურიძე გრიგოლ</v>
+      </c>
+      <c r="C66" t="str">
+        <v>57001010449</v>
+      </c>
+      <c r="E66" t="str">
+        <v>ფიზ. პირი</v>
+      </c>
+      <c r="F66" t="s">
+        <v>54</v>
+      </c>
+      <c r="K66" t="str">
+        <v>GE51BG0000000608679742GEL</v>
+      </c>
+      <c r="S66" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T66" t="s">
+        <v>1786</v>
+      </c>
+      <c r="W66" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:23" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="9"/>
+      <c r="B67" s="10" t="str">
+        <v>სამხრეთის სამშენებლო კომპანია</v>
+      </c>
+      <c r="C67" s="10" t="str">
+        <v>445721595</v>
+      </c>
+      <c r="E67" s="10" t="str">
+        <v xml:space="preserve">შპს </v>
+      </c>
+      <c r="K67" s="10" t="str">
+        <v>GE02BG0000000580784491GEL</v>
+      </c>
+      <c r="S67" s="10" t="s">
+        <v>1782</v>
+      </c>
+      <c r="T67" s="10" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A68" s="2"/>
+    </row>
+    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A69" s="2"/>
+    </row>
+    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A70" s="2"/>
+    </row>
+    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A71" s="2"/>
+    </row>
+    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A72" s="2"/>
+    </row>
+    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A73" s="2"/>
+    </row>
+    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A74" s="2"/>
+    </row>
+    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A75" s="2"/>
+    </row>
+    <row r="76" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A76" s="2"/>
+    </row>
+    <row r="77" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A77" s="2"/>
+    </row>
+    <row r="78" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A78" s="2"/>
+    </row>
+    <row r="79" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A79" s="2"/>
+    </row>
+    <row r="80" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A80" s="2"/>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="2"/>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="2"/>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="2"/>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="2"/>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="2"/>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="2"/>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="2"/>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="2"/>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="2"/>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="2"/>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="2"/>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="2"/>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="2"/>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="2"/>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="2"/>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="2"/>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="2"/>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="2"/>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="2"/>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="2"/>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="2"/>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="2"/>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="2"/>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="2"/>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="2"/>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="2"/>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="2"/>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="2"/>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="2"/>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="2"/>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" s="2"/>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" s="2"/>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="2"/>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" s="2"/>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" s="2"/>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="2"/>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="2"/>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="2"/>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" s="2"/>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="2"/>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" s="2"/>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="2"/>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" s="2"/>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" s="2"/>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" s="2"/>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" s="2"/>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" s="2"/>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" s="2"/>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="2"/>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="2"/>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="2"/>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" s="2"/>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" s="2"/>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" s="2"/>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" s="2"/>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" s="2"/>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="2"/>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" s="2"/>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" s="2"/>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" s="2"/>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" s="2"/>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" s="2"/>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" s="2"/>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" s="2"/>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" s="2"/>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" s="2"/>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" s="2"/>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" s="2"/>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" s="2"/>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" s="2"/>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" s="2"/>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" s="2"/>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" s="2"/>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" s="2"/>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" s="2"/>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" s="2"/>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" s="2"/>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" s="2"/>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" s="2"/>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" s="2"/>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" s="2"/>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" s="2"/>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" s="2"/>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" s="2"/>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" s="2"/>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" s="2"/>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" s="2"/>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" s="2"/>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" s="2"/>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" s="2"/>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" s="2"/>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" s="2"/>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" s="2"/>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" s="2"/>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" s="2"/>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" s="2"/>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" s="2"/>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" s="2"/>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" s="2"/>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" s="2"/>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" s="2"/>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" s="2"/>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" s="2"/>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" s="2"/>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" s="2"/>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" s="2"/>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" s="2"/>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" s="2"/>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" s="2"/>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" s="2"/>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" s="2"/>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" s="2"/>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" s="2"/>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" s="2"/>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" s="2"/>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196" s="2"/>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" s="2"/>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" s="2"/>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199" s="2"/>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200" s="2"/>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201" s="2"/>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202" s="2"/>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203" s="2"/>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204" s="2"/>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A205" s="2"/>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A206" s="2"/>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A207" s="2"/>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A208" s="2"/>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A209" s="2"/>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A210" s="2"/>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A211" s="2"/>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A212" s="2"/>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A213" s="2"/>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A214" s="2"/>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A215" s="2"/>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A216" s="2"/>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A217" s="2"/>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A218" s="2"/>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A219" s="2"/>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A220" s="2"/>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A221" s="2"/>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A222" s="2"/>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A223" s="2"/>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A224" s="2"/>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A225" s="2"/>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A226" s="2"/>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A227" s="2"/>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A228" s="2"/>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A229" s="2"/>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A230" s="2"/>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A231" s="2"/>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A232" s="2"/>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A233" s="2"/>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A234" s="2"/>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A235" s="2"/>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A236" s="2"/>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A237" s="2"/>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A238" s="2"/>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A239" s="2"/>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A240" s="2"/>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A241" s="2"/>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A242" s="2"/>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A243" s="2"/>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A244" s="2"/>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A245" s="2"/>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A246" s="2"/>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A247" s="2"/>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A248" s="2"/>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A249" s="2"/>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A250" s="2"/>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A251" s="2"/>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A252" s="2"/>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A253" s="2"/>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A254" s="2"/>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A255" s="2"/>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A256" s="2"/>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A257" s="2"/>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A258" s="2"/>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A259" s="2"/>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A260" s="2"/>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A261" s="2"/>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A262" s="2"/>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A263" s="2"/>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A264" s="2"/>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A265" s="2"/>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A266" s="2"/>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A267" s="2"/>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A268" s="2"/>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A269" s="2"/>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A270" s="2"/>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A271" s="2"/>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A272" s="2"/>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A273" s="2"/>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A274" s="2"/>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A275" s="2"/>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A276" s="2"/>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A277" s="2"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:Z67" xr:uid="{8E550398-190A-4F15-BF25-77B6E32729EB}">
+    <filterColumn colId="18">
+      <filters>
+        <filter val="e606e963-3d68-4e52-91bd-172b28100c3b"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z277"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T31" sqref="A30:T31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13782,7 +17825,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95703B2E-EFBA-4FCD-899A-4A1547064D72}">
   <dimension ref="A1:AC280"/>
   <sheetViews>
@@ -13973,7 +18016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" ht="315" x14ac:dyDescent="0.25">
       <c r="B4" t="str">
         <f t="shared" si="0"/>
         <v>306282929</v>
@@ -15803,7 +19846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:29" ht="180" x14ac:dyDescent="0.25">
       <c r="B34" t="str">
         <f t="shared" si="0"/>
         <v>01007007062</v>
@@ -15857,7 +19900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:29" ht="195" x14ac:dyDescent="0.25">
       <c r="B35" t="str">
         <f t="shared" si="0"/>
         <v>14001019960</v>

</xml_diff>